<commit_message>
-Add TVS diode -Change the MCU to STM32G0B1CEU6 -Activate the thermal option for the polygon - fix the bom
</commit_message>
<xml_diff>
--- a/Released/BOM/H08R7.xlsx
+++ b/Released/BOM/H08R7.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\HEXABITZ\Modules\Hardware\Modules Hardware Design\H08R7x-Hardware\Released\BOM\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Moazzen\Downloads\Telegram Desktop\H08R7x-Hardware-main\H08R7x-Hardware-main\Released\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{596E4BB3-E78A-4AA6-9C5D-BF79C8F1F4D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15828F5B-CE67-4F1D-9829-9EF95BD04B0D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -127,9 +127,6 @@
     <t>FB1</t>
   </si>
   <si>
-    <t>STM32G0B1CEU6N</t>
-  </si>
-  <si>
     <t>U1</t>
   </si>
   <si>
@@ -139,9 +136,6 @@
     <t>STMicroelectronics</t>
   </si>
   <si>
-    <t>https://octopart.com/stm32g0b1ceu6n-stmicroelectronics-116364672?r=sp</t>
-  </si>
-  <si>
     <t>D1</t>
   </si>
   <si>
@@ -232,9 +226,6 @@
     <t>https://octopart.com/c0603c104k8ractu-kemet-145075?r=sp&amp;s=9bS9ASSwSEqMCE9KBEQZ0g</t>
   </si>
   <si>
-    <t>C3, C5, C6, C8,C10</t>
-  </si>
-  <si>
     <t>R3,R7,R8</t>
   </si>
   <si>
@@ -244,9 +235,6 @@
     <t>https://octopart.com/10tpu4r7msi-panasonic-29487748?r=sp</t>
   </si>
   <si>
-    <t xml:space="preserve"> C7, C4,C11</t>
-  </si>
-  <si>
     <t>TVS DIODE 3,3V 10,9V SOD323</t>
   </si>
   <si>
@@ -290,6 +278,18 @@
   </si>
   <si>
     <t>https://octopart.com/mpz1608s601atd25-tdk-24319482?r=sp</t>
+  </si>
+  <si>
+    <t>C5, C6, C8,C10</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> C7, C11</t>
+  </si>
+  <si>
+    <t>STM32G0B1CEU6</t>
+  </si>
+  <si>
+    <t>https://octopart.com/stm32g0b1ceu6-stmicroelectronics-116363364?r=sp</t>
   </si>
 </sst>
 </file>
@@ -477,7 +477,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -551,6 +551,21 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -571,12 +586,6 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -613,7 +622,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>2174599</xdr:colOff>
+      <xdr:colOff>2326999</xdr:colOff>
       <xdr:row>2</xdr:row>
       <xdr:rowOff>23812</xdr:rowOff>
     </xdr:to>
@@ -955,18 +964,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I23"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D28" sqref="D28"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.69921875" customWidth="1"/>
-    <col min="2" max="2" width="70.59765625" customWidth="1"/>
+    <col min="1" max="1" width="10.69921875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="60.59765625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="21.59765625" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="24.8984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="84" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.3984375" customWidth="1"/>
+    <col min="5" max="5" width="79.69921875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.19921875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="49" customWidth="1"/>
   </cols>
   <sheetData>
@@ -988,7 +997,7 @@
         <v>13</v>
       </c>
       <c r="D2" s="10"/>
-      <c r="E2" s="35" t="s">
+      <c r="E2" s="28" t="s">
         <v>6</v>
       </c>
       <c r="G2" s="7"/>
@@ -1016,11 +1025,11 @@
       <c r="C4" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="27">
+      <c r="D4" s="32">
         <v>0</v>
       </c>
-      <c r="E4" s="27"/>
-      <c r="F4" s="27"/>
+      <c r="E4" s="32"/>
+      <c r="F4" s="32"/>
       <c r="G4" s="2"/>
     </row>
     <row r="5" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
@@ -1028,16 +1037,16 @@
         <v>9</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="D5" s="28">
+      <c r="D5" s="33">
         <v>45375</v>
       </c>
-      <c r="E5" s="29"/>
-      <c r="F5" s="30"/>
+      <c r="E5" s="34"/>
+      <c r="F5" s="35"/>
       <c r="G5" s="2"/>
     </row>
     <row r="6" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
@@ -1045,14 +1054,14 @@
         <v>10</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="C6" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="D6" s="31"/>
-      <c r="E6" s="32"/>
-      <c r="F6" s="33"/>
+      <c r="D6" s="36"/>
+      <c r="E6" s="37"/>
+      <c r="F6" s="38"/>
       <c r="G6" s="2"/>
     </row>
     <row r="8" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
@@ -1080,16 +1089,16 @@
         <v>18</v>
       </c>
       <c r="B9" s="23" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="C9" s="23" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="D9" s="23" t="s">
         <v>19</v>
       </c>
       <c r="E9" s="24" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="F9" s="19">
         <v>1</v>
@@ -1100,7 +1109,7 @@
         <v>20</v>
       </c>
       <c r="B10" s="23" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C10" s="17" t="s">
         <v>21</v>
@@ -1117,30 +1126,30 @@
     </row>
     <row r="11" spans="1:9" s="16" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A11" s="17" t="s">
-        <v>68</v>
+        <v>84</v>
       </c>
       <c r="B11" s="23" t="s">
+        <v>63</v>
+      </c>
+      <c r="C11" s="23" t="s">
+        <v>64</v>
+      </c>
+      <c r="D11" s="23" t="s">
+        <v>62</v>
+      </c>
+      <c r="E11" s="24" t="s">
         <v>65</v>
       </c>
-      <c r="C11" s="23" t="s">
-        <v>66</v>
-      </c>
-      <c r="D11" s="23" t="s">
-        <v>64</v>
-      </c>
-      <c r="E11" s="24" t="s">
-        <v>67</v>
-      </c>
       <c r="F11" s="25">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="12" spans="1:9" s="16" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A12" s="17" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B12" s="26" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C12" s="26" t="s">
         <v>24</v>
@@ -1157,22 +1166,22 @@
     </row>
     <row r="13" spans="1:9" s="16" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A13" s="17" t="s">
-        <v>72</v>
+        <v>85</v>
       </c>
       <c r="B13" s="23" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C13" s="23" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="D13" s="23" t="s">
         <v>16</v>
       </c>
       <c r="E13" s="24" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="F13" s="19">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="14" spans="1:9" s="16" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
@@ -1197,10 +1206,10 @@
     </row>
     <row r="15" spans="1:9" s="16" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A15" s="17" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B15" s="17" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C15" s="18" t="s">
         <v>31</v>
@@ -1209,7 +1218,7 @@
         <v>16</v>
       </c>
       <c r="E15" s="20" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="F15" s="19">
         <v>1</v>
@@ -1217,19 +1226,19 @@
     </row>
     <row r="16" spans="1:9" s="16" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A16" s="17" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B16" s="17" t="s">
+        <v>57</v>
+      </c>
+      <c r="C16" s="17" t="s">
         <v>59</v>
       </c>
-      <c r="C16" s="17" t="s">
-        <v>61</v>
-      </c>
       <c r="D16" s="17" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E16" s="20" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="F16" s="19">
         <v>2</v>
@@ -1237,19 +1246,19 @@
     </row>
     <row r="17" spans="1:6" s="16" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A17" s="17" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="B17" s="18" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C17" s="18" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D17" s="17" t="s">
         <v>28</v>
       </c>
       <c r="E17" s="20" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="F17" s="19">
         <v>3</v>
@@ -1260,16 +1269,16 @@
         <v>32</v>
       </c>
       <c r="B18" s="17" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C18" s="17" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D18" s="17" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E18" s="20" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="F18" s="19">
         <v>1</v>
@@ -1277,79 +1286,79 @@
     </row>
     <row r="19" spans="1:6" s="16" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A19" s="17" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B19" s="17" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="C19" s="17" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="D19" s="17" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E19" s="20" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="F19" s="19">
         <v>1</v>
       </c>
     </row>
     <row r="20" spans="1:6" s="16" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A20" s="17" t="s">
+      <c r="A20" s="29" t="s">
+        <v>33</v>
+      </c>
+      <c r="B20" s="29" t="s">
         <v>34</v>
       </c>
-      <c r="B20" s="17" t="s">
+      <c r="C20" s="29" t="s">
+        <v>86</v>
+      </c>
+      <c r="D20" s="29" t="s">
         <v>35</v>
       </c>
-      <c r="C20" s="17" t="s">
-        <v>33</v>
-      </c>
-      <c r="D20" s="17" t="s">
-        <v>36</v>
-      </c>
-      <c r="E20" s="20" t="s">
-        <v>37</v>
-      </c>
-      <c r="F20" s="19">
+      <c r="E20" s="30" t="s">
+        <v>87</v>
+      </c>
+      <c r="F20" s="31">
         <v>1</v>
       </c>
     </row>
     <row r="21" spans="1:6" s="16" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A21" s="17" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B21" s="17" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C21" s="17" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D21" s="17" t="s">
         <v>17</v>
       </c>
       <c r="E21" s="21" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="F21" s="19">
         <v>1</v>
       </c>
     </row>
     <row r="22" spans="1:6" s="16" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A22" s="34" t="s">
-        <v>77</v>
+      <c r="A22" s="27" t="s">
+        <v>73</v>
       </c>
       <c r="B22" s="17" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="C22" s="17" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="D22" s="17" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="E22" s="21" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="F22" s="19">
         <v>1</v>
@@ -1357,19 +1366,19 @@
     </row>
     <row r="23" spans="1:6" s="16" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A23" s="22" t="s">
+        <v>38</v>
+      </c>
+      <c r="B23" s="17" t="s">
+        <v>39</v>
+      </c>
+      <c r="C23" s="17" t="s">
         <v>40</v>
-      </c>
-      <c r="B23" s="17" t="s">
-        <v>41</v>
-      </c>
-      <c r="C23" s="17" t="s">
-        <v>42</v>
       </c>
       <c r="D23" s="17" t="s">
         <v>15</v>
       </c>
       <c r="E23" s="20" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="F23" s="19">
         <v>1</v>
@@ -1383,16 +1392,16 @@
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="E14" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
-    <hyperlink ref="E20" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
-    <hyperlink ref="E23" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
-    <hyperlink ref="D21" r:id="rId4" display="https://octopart.com/manufacturers/wolfspeed" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
-    <hyperlink ref="E10" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
-    <hyperlink ref="E21" r:id="rId6" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
-    <hyperlink ref="E15" r:id="rId7" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
-    <hyperlink ref="E11" r:id="rId8" xr:uid="{663B604C-0778-4D31-8D01-1E3B83AE8D9B}"/>
-    <hyperlink ref="E13" r:id="rId9" xr:uid="{23CC8D52-00B7-424D-AE6F-D90CF0F8A6D7}"/>
-    <hyperlink ref="E12" r:id="rId10" xr:uid="{636BB640-56DA-4B3A-8EBB-00A74F7EF75D}"/>
-    <hyperlink ref="E16" r:id="rId11" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
+    <hyperlink ref="E23" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="D21" r:id="rId3" display="https://octopart.com/manufacturers/wolfspeed" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="E10" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="E21" r:id="rId5" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
+    <hyperlink ref="E15" r:id="rId6" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
+    <hyperlink ref="E11" r:id="rId7" xr:uid="{663B604C-0778-4D31-8D01-1E3B83AE8D9B}"/>
+    <hyperlink ref="E13" r:id="rId8" xr:uid="{23CC8D52-00B7-424D-AE6F-D90CF0F8A6D7}"/>
+    <hyperlink ref="E12" r:id="rId9" xr:uid="{636BB640-56DA-4B3A-8EBB-00A74F7EF75D}"/>
+    <hyperlink ref="E16" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
+    <hyperlink ref="E20" r:id="rId11" xr:uid="{291BF8FA-EE38-4DF7-BF93-B45CF00DEE2B}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId12"/>

</xml_diff>